<commit_message>
Restructuring of the tree
</commit_message>
<xml_diff>
--- a/data/complete_tree/A11_weights.xlsx
+++ b/data/complete_tree/A11_weights.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikonagengast/Desktop/Paper_MA/Paper_Recycling_3/AHP_Monte_Carlo/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikonagengast/Desktop/Paper_MA/Paper_Recycling_3/AHP_Monte_Carlo/data/complete_tree/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{91CEF264-56D2-674D-86D0-ADC43957E63E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C13C4749-2894-8243-8C48-CDDA4A848C6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="11460" yWindow="500" windowWidth="19360" windowHeight="18440" xr2:uid="{B7E2081D-577B-684F-9742-E21C9EA83400}"/>
   </bookViews>
@@ -33,12 +33,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="3">
   <si>
     <t>B</t>
   </si>
   <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>D</t>
   </si>
 </sst>
 </file>
@@ -74,9 +77,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -391,34 +393,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D811DF9-B900-C742-ABBA-AD4B5390F82E}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>0</v>
       </c>
       <c r="C1" t="s">
         <v>1</v>
       </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
         <v>0.2</v>
       </c>
+      <c r="D2">
+        <v>0.2</v>
+      </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -426,6 +434,23 @@
         <v>5</v>
       </c>
       <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>5</v>
+      </c>
+      <c r="D4">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adjustment of weight matrizes
</commit_message>
<xml_diff>
--- a/data/complete_tree/A11_weights.xlsx
+++ b/data/complete_tree/A11_weights.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nikonagengast/Desktop/Paper_MA/Paper_Recycling_3/AHP_Monte_Carlo/data/complete_tree/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C13C4749-2894-8243-8C48-CDDA4A848C6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C689723-4ED4-134F-8FCD-69EE9E81B338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11460" yWindow="500" windowWidth="19360" windowHeight="18440" xr2:uid="{B7E2081D-577B-684F-9742-E21C9EA83400}"/>
+    <workbookView xWindow="16020" yWindow="2560" windowWidth="19360" windowHeight="18440" xr2:uid="{B7E2081D-577B-684F-9742-E21C9EA83400}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,14 +19,6 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -396,7 +388,7 @@
   <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -423,7 +415,7 @@
         <v>0.2</v>
       </c>
       <c r="D2">
-        <v>0.2</v>
+        <v>0.11</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -437,7 +429,7 @@
         <v>1</v>
       </c>
       <c r="D3">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -445,10 +437,10 @@
         <v>2</v>
       </c>
       <c r="B4">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D4">
         <v>1</v>

</xml_diff>